<commit_message>
updated mappings to remove IEX key stats where data was erroneous
</commit_message>
<xml_diff>
--- a/Valuations.xlsx
+++ b/Valuations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="1050" windowWidth="12408" windowHeight="9258" activeTab="2"/>
+    <workbookView xWindow="5880" yWindow="1054" windowWidth="12411" windowHeight="9257" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="239">
   <si>
     <t>Name</t>
   </si>
@@ -728,6 +728,12 @@
   </si>
   <si>
     <t>IEX ('Key Stats')</t>
+  </si>
+  <si>
+    <t>IEX ('earnings')</t>
+  </si>
+  <si>
+    <t>IEX ('financials')</t>
   </si>
 </sst>
 </file>
@@ -790,7 +796,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -836,12 +842,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -926,11 +947,17 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -941,12 +968,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1271,16 +1295,16 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.578125" customWidth="1"/>
-    <col min="7" max="7" width="33.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.53515625" customWidth="1"/>
+    <col min="7" max="7" width="33.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1300,40 +1324,40 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="68" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="71" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="68"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="71"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="68"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="71"/>
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="68"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="71"/>
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="68"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="71"/>
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="68"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="71"/>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1350,8 +1374,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="68"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="71"/>
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -1359,8 +1383,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="68" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="71" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1376,8 +1400,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="68"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="71"/>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1385,8 +1409,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="68"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="71"/>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1394,8 +1418,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="68" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="71" t="s">
         <v>48</v>
       </c>
       <c r="B12" t="s">
@@ -1408,8 +1432,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="68"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="71"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -1417,8 +1441,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="68"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="71"/>
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -1429,8 +1453,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="68"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="71"/>
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -1438,8 +1462,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="68"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="71"/>
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -1453,8 +1477,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="68"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="71"/>
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -1465,8 +1489,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="68"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="71"/>
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -1535,7 +1559,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -1565,7 +1589,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>27</v>
       </c>
@@ -1573,7 +1597,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>28</v>
       </c>
@@ -1590,7 +1614,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>29</v>
       </c>
@@ -1604,7 +1628,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>30</v>
       </c>
@@ -1628,35 +1652,35 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A1" s="71" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69" t="s">
+      <c r="F1" s="72"/>
+      <c r="G1" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="69"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="68"/>
+      <c r="H1" s="72"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" s="71"/>
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1670,8 +1694,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="68"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="71"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1685,8 +1709,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="68"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" s="71"/>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1697,41 +1721,41 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="68"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" s="71"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="G5" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="69"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="68"/>
+      <c r="H5" s="72"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" s="71"/>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="69"/>
+      <c r="F6" s="72"/>
       <c r="G6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="68"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" s="71"/>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="69"/>
+      <c r="D7" s="72"/>
       <c r="E7" t="s">
         <v>11</v>
       </c>
@@ -1739,8 +1763,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="68"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" s="71"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1754,8 +1778,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="68" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" s="71" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1771,8 +1795,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="68"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="71"/>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1783,8 +1807,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="68"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" s="71"/>
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1794,13 +1818,13 @@
       <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="69" t="s">
+      <c r="G11" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="69"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="68" t="s">
+      <c r="H11" s="72"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12" s="71" t="s">
         <v>48</v>
       </c>
       <c r="B12" t="s">
@@ -1816,8 +1840,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="68"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A13" s="71"/>
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -1831,8 +1855,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="68"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A14" s="71"/>
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -1843,8 +1867,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="68"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A15" s="71"/>
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -1852,8 +1876,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="68"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A16" s="71"/>
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -1861,8 +1885,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="68"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="71"/>
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -1870,8 +1894,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="68"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="71"/>
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -1879,8 +1903,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="68" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="71" t="s">
         <v>62</v>
       </c>
       <c r="B19" t="s">
@@ -1890,8 +1914,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="68"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" s="71"/>
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -1899,78 +1923,78 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="68"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" s="71"/>
       <c r="B21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="68" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22" s="71" t="s">
         <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="68"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A23" s="71"/>
       <c r="B23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="68"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24" s="71"/>
       <c r="B24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="68"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" s="71"/>
       <c r="B25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="68" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="71" t="s">
         <v>68</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="68"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="71"/>
       <c r="B27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="68"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="71"/>
       <c r="B28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="68"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="71"/>
       <c r="B29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="68"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="71"/>
       <c r="B30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="68"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="71"/>
       <c r="B31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="68"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" s="71"/>
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -1998,37 +2022,37 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.15625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.15234375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>230</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="68" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="69" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="69" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="68" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A2" s="71" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
@@ -2042,8 +2066,8 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="68"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A3" s="71"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -2053,8 +2077,8 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="68"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A4" s="71"/>
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -2062,12 +2086,12 @@
         <v>108</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="70" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="68"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A5" s="71"/>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -2079,8 +2103,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="68"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A6" s="71"/>
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -2088,13 +2112,13 @@
         <v>108</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="70" t="s">
         <v>236</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="68"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A7" s="71"/>
       <c r="B7" t="s">
         <v>140</v>
       </c>
@@ -2106,16 +2130,16 @@
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="68"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A8" s="71"/>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="68"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A9" s="71"/>
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -2123,49 +2147,61 @@
         <v>141</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="70" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="75" t="s">
+      <c r="H9" s="77">
+        <v>0.48</v>
+      </c>
+      <c r="I9" s="77">
+        <v>-1.78</v>
+      </c>
+      <c r="J9" s="77">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K9" s="77">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A10" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76" t="s">
+      <c r="D10" s="70"/>
+      <c r="E10" s="70" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="75"/>
-      <c r="B11" s="76" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11" s="73"/>
+      <c r="B11" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="75"/>
-      <c r="B12" s="76" t="s">
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A12" s="73"/>
+      <c r="B12" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="68" t="s">
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A13" s="71" t="s">
         <v>48</v>
       </c>
       <c r="B13" t="s">
@@ -2177,12 +2213,12 @@
       <c r="D13" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="70" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="68"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A14" s="71"/>
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -2190,12 +2226,12 @@
         <v>141</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="76" t="s">
+      <c r="E14" s="70" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="68"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A15" s="71"/>
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -2203,12 +2239,12 @@
         <v>141</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="76" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="68"/>
+      <c r="E15" s="70" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A16" s="71"/>
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2216,12 +2252,12 @@
         <v>108</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="76" t="s">
+      <c r="E16" s="70" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="68"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="71"/>
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -2229,76 +2265,84 @@
         <v>141</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="76" t="s">
+      <c r="E17" s="70" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="68"/>
+      <c r="I17">
+        <f>AVERAGE(H9:K9)</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" s="71"/>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="76" t="s">
+      <c r="E18" s="70" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="68"/>
+      <c r="I18">
+        <f>AVERAGE(I9:K9)</f>
+        <v>-0.14666666666666664</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" s="71"/>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="75" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="75"/>
-      <c r="B21" s="76" t="s">
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21" s="73"/>
+      <c r="B21" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="75"/>
-      <c r="B22" s="76" t="s">
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22" s="73"/>
+      <c r="B22" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="76" t="s">
+      <c r="C22" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D22" s="76" t="s">
+      <c r="D22" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="E22" s="76"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="75"/>
-      <c r="B23" s="76" t="s">
+      <c r="E22" s="70"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23" s="73"/>
+      <c r="B23" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="76" t="s">
+      <c r="C23" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="76" t="s">
+      <c r="D23" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="E23" s="76"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="68" t="s">
+      <c r="E23" s="70"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A24" s="71" t="s">
         <v>67</v>
       </c>
       <c r="B24" t="s">
@@ -2307,16 +2351,16 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="68"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25" s="71"/>
       <c r="B25" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="68"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" s="71"/>
       <c r="B26" t="s">
         <v>23</v>
       </c>
@@ -2324,8 +2368,8 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="68"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A27" s="71"/>
       <c r="B27" t="s">
         <v>24</v>
       </c>
@@ -2333,104 +2377,104 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="75" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A28" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="76" t="s">
+      <c r="C28" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="76" t="s">
+      <c r="D28" s="70" t="s">
         <v>198</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="75"/>
-      <c r="B29" s="76" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A29" s="73"/>
+      <c r="B29" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="76" t="s">
+      <c r="C29" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="76" t="s">
+      <c r="D29" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="E29" s="76"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="75"/>
-      <c r="B30" s="76" t="s">
+      <c r="E29" s="70"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30" s="73"/>
+      <c r="B30" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="76" t="s">
+      <c r="C30" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D30" s="76" t="s">
+      <c r="D30" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="E30" s="76" t="s">
+      <c r="E30" s="70" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="75"/>
-      <c r="B31" s="76" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31" s="73"/>
+      <c r="B31" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="76" t="s">
+      <c r="C31" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D31" s="76" t="s">
+      <c r="D31" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="E31" s="76" t="s">
+      <c r="E31" s="70" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="75"/>
-      <c r="B32" s="76" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32" s="73"/>
+      <c r="B32" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="76" t="s">
+      <c r="C32" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="75"/>
-      <c r="B33" s="76" t="s">
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A33" s="73"/>
+      <c r="B33" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="76" t="s">
+      <c r="C33" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="75"/>
-      <c r="B34" s="76" t="s">
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A34" s="73"/>
+      <c r="B34" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="76" t="s">
+      <c r="C34" s="70" t="s">
         <v>199</v>
       </c>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35" s="76"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B35" s="70"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
@@ -2457,35 +2501,35 @@
       <selection pane="topRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.83984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.41796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.15625" style="5"/>
-    <col min="10" max="10" width="13.15625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.15625" style="8"/>
-    <col min="12" max="12" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.84375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3828125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.15234375" style="5"/>
+    <col min="10" max="10" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.15234375" style="8"/>
+    <col min="12" max="12" width="12.23046875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="8" customWidth="1"/>
-    <col min="14" max="14" width="13.15625" customWidth="1"/>
-    <col min="15" max="15" width="16.26171875" style="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.15234375" customWidth="1"/>
+    <col min="15" max="15" width="16.23046875" style="39" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" style="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.15625" style="5"/>
-    <col min="20" max="20" width="9.15625" style="5"/>
-    <col min="21" max="21" width="9.15625" style="29"/>
-    <col min="22" max="22" width="15.68359375" style="30" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.26171875" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.15625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.83984375" style="48" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.15625" style="52"/>
+    <col min="18" max="18" width="9.15234375" style="5"/>
+    <col min="20" max="20" width="9.15234375" style="5"/>
+    <col min="21" max="21" width="9.15234375" style="29"/>
+    <col min="22" max="22" width="15.69140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.23046875" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.15234375" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.84375" style="48" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.15234375" style="52"/>
     <col min="29" max="29" width="14" style="57" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.15625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.68359375" style="61" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.3671875" style="8" customWidth="1"/>
-    <col min="34" max="34" width="13.734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.15234375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.69140625" style="61" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.3828125" style="8" customWidth="1"/>
+    <col min="34" max="34" width="13.765625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="15" x14ac:dyDescent="0.25">
@@ -2547,21 +2591,21 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="68" t="s">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A3" s="71" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="F3" s="70" t="s">
+      <c r="D3" s="76"/>
+      <c r="F3" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="71"/>
+      <c r="G3" s="75"/>
       <c r="H3" t="s">
         <v>101</v>
       </c>
@@ -2611,19 +2655,19 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="68"/>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A4" s="71"/>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="72"/>
-      <c r="F4" s="70" t="s">
+      <c r="D4" s="76"/>
+      <c r="F4" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="71"/>
+      <c r="G4" s="75"/>
       <c r="H4" t="s">
         <v>102</v>
       </c>
@@ -2689,8 +2733,8 @@
       <c r="AK4" s="14"/>
       <c r="AL4" s="14"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="68"/>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A5" s="71"/>
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -2752,8 +2796,8 @@
         <v>159.99</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="68"/>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A6" s="71"/>
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -2815,8 +2859,8 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="68"/>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A7" s="71"/>
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -2872,8 +2916,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="68"/>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A8" s="71"/>
       <c r="B8" t="s">
         <v>139</v>
       </c>
@@ -2882,8 +2926,8 @@
         <v>794506.86713999999</v>
       </c>
     </row>
-    <row r="9" spans="1:38" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="68"/>
+    <row r="9" spans="1:38" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="71"/>
       <c r="B9" s="18" t="s">
         <v>6</v>
       </c>
@@ -2958,8 +3002,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="68" t="s">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A10" s="71" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -3040,8 +3084,8 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="11" spans="1:38" s="22" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="68"/>
+    <row r="11" spans="1:38" s="22" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="71"/>
       <c r="B11" s="21" t="s">
         <v>8</v>
       </c>
@@ -3115,8 +3159,8 @@
         <v>2329</v>
       </c>
     </row>
-    <row r="12" spans="1:38" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="68"/>
+    <row r="12" spans="1:38" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="71"/>
       <c r="B12" s="25" t="s">
         <v>9</v>
       </c>
@@ -3202,8 +3246,8 @@
         <v>723</v>
       </c>
     </row>
-    <row r="13" spans="1:38" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="68" t="s">
+    <row r="13" spans="1:38" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="71" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="26" t="s">
@@ -3283,8 +3327,8 @@
         <v>12.557490144546648</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="68"/>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A14" s="71"/>
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -3359,8 +3403,8 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="68"/>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A15" s="71"/>
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -3432,8 +3476,8 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="68"/>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A16" s="71"/>
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -3495,8 +3539,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="68"/>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A17" s="71"/>
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -3571,8 +3615,8 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="68"/>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A18" s="71"/>
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -3622,8 +3666,8 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="68" t="s">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A19" s="71" t="s">
         <v>62</v>
       </c>
       <c r="B19" t="s">
@@ -3641,8 +3685,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="68"/>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A20" s="71"/>
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -3650,8 +3694,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="68"/>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A21" s="71"/>
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -3659,8 +3703,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="68"/>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A22" s="71"/>
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -3716,8 +3760,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="68" t="s">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A23" s="71" t="s">
         <v>67</v>
       </c>
       <c r="B23" t="s">
@@ -3761,8 +3805,8 @@
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="68"/>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A24" s="71"/>
       <c r="B24" t="s">
         <v>21</v>
       </c>
@@ -3788,22 +3832,22 @@
       </c>
       <c r="U24" s="38"/>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="68"/>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A25" s="71"/>
       <c r="B25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="68" t="s">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A26" s="71" t="s">
         <v>68</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="68"/>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A27" s="71"/>
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -3856,8 +3900,8 @@
         <v>11.48</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="68"/>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A28" s="71"/>
       <c r="B28" t="s">
         <v>69</v>
       </c>
@@ -3898,8 +3942,8 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="68"/>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A29" s="71"/>
       <c r="B29" t="s">
         <v>26</v>
       </c>
@@ -3955,8 +3999,8 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="68"/>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A30" s="71"/>
       <c r="B30" t="s">
         <v>27</v>
       </c>
@@ -4016,8 +4060,8 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="68"/>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A31" s="71"/>
       <c r="B31" t="s">
         <v>28</v>
       </c>
@@ -4073,8 +4117,8 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="68"/>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A32" s="71"/>
       <c r="B32" t="s">
         <v>29</v>
       </c>
@@ -4130,13 +4174,13 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="68"/>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A33" s="71"/>
       <c r="B33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.4">
       <c r="L35" s="10"/>
       <c r="M35" s="13"/>
       <c r="N35" s="10"/>
@@ -4144,7 +4188,7 @@
       <c r="P35" s="46"/>
       <c r="Q35" s="10"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10">

</xml_diff>